<commit_message>
Added members with no wars
</commit_message>
<xml_diff>
--- a/docs/data/warstats.xlsx
+++ b/docs/data/warstats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -59,36 +59,36 @@
     <t>Fabíola</t>
   </si>
   <si>
+    <t>leal</t>
+  </si>
+  <si>
+    <t>Goblyn</t>
+  </si>
+  <si>
+    <t>Inferno</t>
+  </si>
+  <si>
+    <t>snowkids</t>
+  </si>
+  <si>
+    <t>Madnasty</t>
+  </si>
+  <si>
     <t>Robb Stark</t>
   </si>
   <si>
-    <t>leal</t>
-  </si>
-  <si>
-    <t>Goblyn</t>
-  </si>
-  <si>
-    <t>Inferno</t>
-  </si>
-  <si>
-    <t>snowkids</t>
-  </si>
-  <si>
-    <t>Madnasty</t>
-  </si>
-  <si>
     <t>King Bonixe</t>
   </si>
   <si>
     <t>zau</t>
   </si>
   <si>
+    <t>unb</t>
+  </si>
+  <si>
     <t>pjp</t>
   </si>
   <si>
-    <t>unb</t>
-  </si>
-  <si>
     <t>faneca</t>
   </si>
   <si>
@@ -101,12 +101,12 @@
     <t>TheKingJK</t>
   </si>
   <si>
+    <t>Ricky</t>
+  </si>
+  <si>
     <t>filipe</t>
   </si>
   <si>
-    <t>Ricky</t>
-  </si>
-  <si>
     <t>carmen</t>
   </si>
   <si>
@@ -125,15 +125,15 @@
     <t>Tabo da amarela</t>
   </si>
   <si>
+    <t>Matilde Pires</t>
+  </si>
+  <si>
+    <t>Savler</t>
+  </si>
+  <si>
     <t>YOSHINZ</t>
   </si>
   <si>
-    <t>Matilde Pires</t>
-  </si>
-  <si>
-    <t>Savler</t>
-  </si>
-  <si>
     <t>Welton</t>
   </si>
   <si>
@@ -146,27 +146,24 @@
     <t>hugo</t>
   </si>
   <si>
+    <t>Sergas</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Manu</t>
+  </si>
+  <si>
+    <t>mounir</t>
+  </si>
+  <si>
     <t>Pikaya</t>
   </si>
   <si>
-    <t>Sergas</t>
-  </si>
-  <si>
-    <t>Marcelo</t>
-  </si>
-  <si>
-    <t>mounir</t>
-  </si>
-  <si>
-    <t>Manu</t>
-  </si>
-  <si>
     <t>supercell</t>
   </si>
   <si>
-    <t>castelhano</t>
-  </si>
-  <si>
     <t>NOVA I MIGUEL☉</t>
   </si>
   <si>
@@ -176,7 +173,7 @@
     <t>Sra. Clash</t>
   </si>
   <si>
-    <t>Alex</t>
+    <t>SELFIE</t>
   </si>
   <si>
     <t>MASTER PT</t>
@@ -279,19 +276,19 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C2" t="n">
-        <v>78.0</v>
+        <v>81.0</v>
       </c>
       <c r="D2" t="n">
-        <v>31920.0</v>
+        <v>33320.0</v>
       </c>
       <c r="E2" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="F2" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -300,10 +297,10 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>82.0</v>
+        <v>83.0</v>
       </c>
       <c r="J2" t="n">
-        <v>260.0</v>
+        <v>269.0</v>
       </c>
     </row>
     <row r="3">
@@ -311,19 +308,19 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C3" t="n">
-        <v>78.0</v>
+        <v>81.0</v>
       </c>
       <c r="D3" t="n">
-        <v>30520.0</v>
+        <v>31920.0</v>
       </c>
       <c r="E3" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="F3" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -332,10 +329,10 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>79.0</v>
+        <v>80.0</v>
       </c>
       <c r="J3" t="n">
-        <v>252.0</v>
+        <v>261.0</v>
       </c>
     </row>
     <row r="4">
@@ -343,19 +340,19 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C4" t="n">
-        <v>78.0</v>
+        <v>81.0</v>
       </c>
       <c r="D4" t="n">
-        <v>31920.0</v>
+        <v>33040.0</v>
       </c>
       <c r="E4" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="F4" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -364,10 +361,10 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>75.0</v>
+        <v>76.0</v>
       </c>
       <c r="J4" t="n">
-        <v>232.0</v>
+        <v>241.0</v>
       </c>
     </row>
     <row r="5">
@@ -375,19 +372,19 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C5" t="n">
-        <v>78.0</v>
+        <v>81.0</v>
       </c>
       <c r="D5" t="n">
-        <v>34440.0</v>
+        <v>35840.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="F5" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -396,10 +393,10 @@
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>64.0</v>
+        <v>66.0</v>
       </c>
       <c r="J5" t="n">
-        <v>212.0</v>
+        <v>221.0</v>
       </c>
     </row>
     <row r="6">
@@ -407,19 +404,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C6" t="n">
-        <v>75.0</v>
+        <v>78.0</v>
       </c>
       <c r="D6" t="n">
-        <v>28735.0</v>
+        <v>29855.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="F6" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -428,10 +425,10 @@
         <v>0.0</v>
       </c>
       <c r="I6" t="n">
-        <v>65.0</v>
+        <v>67.0</v>
       </c>
       <c r="J6" t="n">
-        <v>207.0</v>
+        <v>216.0</v>
       </c>
     </row>
     <row r="7">
@@ -442,28 +439,28 @@
         <v>25.0</v>
       </c>
       <c r="C7" t="n">
-        <v>75.0</v>
+        <v>73.0</v>
       </c>
       <c r="D7" t="n">
-        <v>29082.0</v>
+        <v>29400.0</v>
       </c>
       <c r="E7" t="n">
         <v>25.0</v>
       </c>
       <c r="F7" t="n">
-        <v>16.0</v>
+        <v>19.0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>64.0</v>
+        <v>76.0</v>
       </c>
       <c r="J7" t="n">
-        <v>206.0</v>
+        <v>214.0</v>
       </c>
     </row>
     <row r="8">
@@ -471,31 +468,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="C8" t="n">
-        <v>70.0</v>
+        <v>81.0</v>
       </c>
       <c r="D8" t="n">
-        <v>27720.0</v>
+        <v>33320.0</v>
       </c>
       <c r="E8" t="n">
-        <v>24.0</v>
+        <v>29.0</v>
       </c>
       <c r="F8" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="G8" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
       </c>
       <c r="I8" t="n">
-        <v>75.0</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>205.0</v>
+        <v>211.0</v>
       </c>
     </row>
     <row r="9">
@@ -503,31 +500,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>31372.0</v>
+      </c>
+      <c r="E9" t="n">
         <v>26.0</v>
       </c>
-      <c r="C9" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>32200.0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>28.0</v>
-      </c>
       <c r="F9" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I9" t="n">
-        <v>54.0</v>
+        <v>73.0</v>
       </c>
       <c r="J9" t="n">
-        <v>202.0</v>
+        <v>210.0</v>
       </c>
     </row>
     <row r="10">
@@ -535,31 +532,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C10" t="n">
-        <v>78.0</v>
+        <v>79.0</v>
       </c>
       <c r="D10" t="n">
-        <v>30252.0</v>
+        <v>31690.0</v>
       </c>
       <c r="E10" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="F10" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10" t="n">
-        <v>72.0</v>
+        <v>56.99999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>202.0</v>
+        <v>204.0</v>
       </c>
     </row>
     <row r="11">
@@ -567,31 +564,31 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
       <c r="C11" t="n">
-        <v>76.0</v>
+        <v>75.0</v>
       </c>
       <c r="D11" t="n">
-        <v>30290.0</v>
+        <v>29120.0</v>
       </c>
       <c r="E11" t="n">
         <v>27.0</v>
       </c>
       <c r="F11" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="n">
         <v>0.0</v>
       </c>
       <c r="I11" t="n">
-        <v>56.00000000000001</v>
+        <v>59.0</v>
       </c>
       <c r="J11" t="n">
-        <v>194.0</v>
+        <v>198.0</v>
       </c>
     </row>
     <row r="12">
@@ -599,31 +596,31 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
       <c r="C12" t="n">
-        <v>72.0</v>
+        <v>78.0</v>
       </c>
       <c r="D12" t="n">
-        <v>27720.0</v>
+        <v>30202.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
       <c r="F12" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I12" t="n">
-        <v>57.99999999999999</v>
+        <v>64.0</v>
       </c>
       <c r="J12" t="n">
-        <v>189.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="13">
@@ -631,19 +628,19 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="C13" t="n">
-        <v>63.0</v>
+        <v>66.0</v>
       </c>
       <c r="D13" t="n">
-        <v>25200.0</v>
+        <v>26600.0</v>
       </c>
       <c r="E13" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="F13" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G13" t="n">
         <v>3.0</v>
@@ -652,10 +649,10 @@
         <v>0.0</v>
       </c>
       <c r="I13" t="n">
-        <v>60.0</v>
+        <v>62.0</v>
       </c>
       <c r="J13" t="n">
-        <v>184.0</v>
+        <v>193.0</v>
       </c>
     </row>
     <row r="14">
@@ -663,19 +660,19 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C14" t="n">
-        <v>76.0</v>
+        <v>79.0</v>
       </c>
       <c r="D14" t="n">
-        <v>31080.0</v>
+        <v>32760.0</v>
       </c>
       <c r="E14" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="F14" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="G14" t="n">
         <v>2.0</v>
@@ -684,10 +681,10 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>48.0</v>
+        <v>50.0</v>
       </c>
       <c r="J14" t="n">
-        <v>183.0</v>
+        <v>192.0</v>
       </c>
     </row>
     <row r="15">
@@ -695,31 +692,31 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="C15" t="n">
-        <v>71.0</v>
+        <v>66.0</v>
       </c>
       <c r="D15" t="n">
-        <v>28560.0</v>
+        <v>27720.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
       <c r="F15" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>48.0</v>
+        <v>74.0</v>
       </c>
       <c r="J15" t="n">
-        <v>176.0</v>
+        <v>179.0</v>
       </c>
     </row>
     <row r="16">
@@ -727,31 +724,31 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="C16" t="n">
-        <v>63.0</v>
+        <v>74.0</v>
       </c>
       <c r="D16" t="n">
-        <v>26600.0</v>
+        <v>29400.0</v>
       </c>
       <c r="E16" t="n">
-        <v>22.0</v>
+        <v>26.0</v>
       </c>
       <c r="F16" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H16" t="n">
         <v>0.0</v>
       </c>
       <c r="I16" t="n">
-        <v>73.0</v>
+        <v>46.0</v>
       </c>
       <c r="J16" t="n">
-        <v>171.0</v>
+        <v>178.0</v>
       </c>
     </row>
     <row r="17">
@@ -759,16 +756,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="C17" t="n">
-        <v>77.0</v>
+        <v>80.0</v>
       </c>
       <c r="D17" t="n">
-        <v>28779.0</v>
+        <v>30249.0</v>
       </c>
       <c r="E17" t="n">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="F17" t="n">
         <v>13.0</v>
@@ -780,10 +777,10 @@
         <v>0.0</v>
       </c>
       <c r="I17" t="n">
-        <v>43.0</v>
+        <v>42.0</v>
       </c>
       <c r="J17" t="n">
-        <v>170.0</v>
+        <v>174.0</v>
       </c>
     </row>
     <row r="18">
@@ -791,16 +788,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C18" t="n">
-        <v>75.0</v>
+        <v>78.0</v>
       </c>
       <c r="D18" t="n">
-        <v>29411.0</v>
+        <v>30531.0</v>
       </c>
       <c r="E18" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="F18" t="n">
         <v>12.0</v>
@@ -812,10 +809,10 @@
         <v>0.0</v>
       </c>
       <c r="I18" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="J18" t="n">
-        <v>168.0</v>
+        <v>171.0</v>
       </c>
     </row>
     <row r="19">
@@ -823,19 +820,19 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="C19" t="n">
-        <v>69.0</v>
+        <v>72.0</v>
       </c>
       <c r="D19" t="n">
-        <v>26347.0</v>
+        <v>27467.0</v>
       </c>
       <c r="E19" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="F19" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -844,10 +841,10 @@
         <v>1.0</v>
       </c>
       <c r="I19" t="n">
-        <v>61.0</v>
+        <v>62.0</v>
       </c>
       <c r="J19" t="n">
-        <v>158.0</v>
+        <v>166.0</v>
       </c>
     </row>
     <row r="20">
@@ -855,16 +852,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C20" t="n">
-        <v>57.0</v>
+        <v>60.0</v>
       </c>
       <c r="D20" t="n">
-        <v>24640.0</v>
+        <v>25760.0</v>
       </c>
       <c r="E20" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="F20" t="n">
         <v>12.0</v>
@@ -876,10 +873,10 @@
         <v>0.0</v>
       </c>
       <c r="I20" t="n">
-        <v>52.0</v>
+        <v>50.0</v>
       </c>
       <c r="J20" t="n">
-        <v>149.0</v>
+        <v>152.0</v>
       </c>
     </row>
     <row r="21">
@@ -887,31 +884,31 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>24.0</v>
+        <v>23.0</v>
       </c>
       <c r="C21" t="n">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="D21" t="n">
-        <v>28560.0</v>
+        <v>24768.0</v>
       </c>
       <c r="E21" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="F21" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G21" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="H21" t="n">
         <v>0.0</v>
       </c>
       <c r="I21" t="n">
-        <v>46.0</v>
+        <v>40.0</v>
       </c>
       <c r="J21" t="n">
-        <v>144.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="22">
@@ -919,31 +916,31 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="C22" t="n">
-        <v>63.0</v>
+        <v>68.0</v>
       </c>
       <c r="D22" t="n">
-        <v>23719.0</v>
+        <v>29680.0</v>
       </c>
       <c r="E22" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="F22" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="G22" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="H22" t="n">
         <v>0.0</v>
       </c>
       <c r="I22" t="n">
-        <v>38.0</v>
+        <v>44.0</v>
       </c>
       <c r="J22" t="n">
-        <v>142.0</v>
+        <v>147.0</v>
       </c>
     </row>
     <row r="23">
@@ -951,16 +948,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C23" t="n">
-        <v>74.0</v>
+        <v>77.0</v>
       </c>
       <c r="D23" t="n">
-        <v>26694.0</v>
+        <v>27743.0</v>
       </c>
       <c r="E23" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="F23" t="n">
         <v>9.0</v>
@@ -972,10 +969,10 @@
         <v>0.0</v>
       </c>
       <c r="I23" t="n">
-        <v>33.0</v>
+        <v>32.0</v>
       </c>
       <c r="J23" t="n">
-        <v>138.0</v>
+        <v>141.0</v>
       </c>
     </row>
     <row r="24">
@@ -983,19 +980,19 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="C24" t="n">
-        <v>72.0</v>
+        <v>75.0</v>
       </c>
       <c r="D24" t="n">
-        <v>26070.0</v>
+        <v>27540.0</v>
       </c>
       <c r="E24" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="F24" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="G24" t="n">
         <v>0.0</v>
@@ -1004,10 +1001,10 @@
         <v>0.0</v>
       </c>
       <c r="I24" t="n">
-        <v>28.000000000000004</v>
+        <v>31.0</v>
       </c>
       <c r="J24" t="n">
-        <v>126.0</v>
+        <v>136.0</v>
       </c>
     </row>
     <row r="25">
@@ -1015,16 +1012,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>26040.0</v>
+      </c>
+      <c r="E25" t="n">
         <v>23.0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>63.0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>24920.0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>22.0</v>
       </c>
       <c r="F25" t="n">
         <v>16.0</v>
@@ -1036,10 +1033,10 @@
         <v>2.0</v>
       </c>
       <c r="I25" t="n">
-        <v>73.0</v>
+        <v>70.0</v>
       </c>
       <c r="J25" t="n">
-        <v>119.0</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="26">
@@ -1079,16 +1076,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C27" t="n">
-        <v>70.0</v>
+        <v>73.0</v>
       </c>
       <c r="D27" t="n">
-        <v>28413.0</v>
+        <v>29199.0</v>
       </c>
       <c r="E27" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="F27" t="n">
         <v>8.0</v>
@@ -1100,10 +1097,10 @@
         <v>2.0</v>
       </c>
       <c r="I27" t="n">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="J27" t="n">
-        <v>108.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="28">
@@ -1111,16 +1108,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C28" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="D28" t="n">
-        <v>5040.0</v>
+        <v>6440.0</v>
       </c>
       <c r="E28" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="F28" t="n">
         <v>3.0</v>
@@ -1132,10 +1129,10 @@
         <v>0.0</v>
       </c>
       <c r="I28" t="n">
-        <v>75.0</v>
+        <v>60.0</v>
       </c>
       <c r="J28" t="n">
-        <v>95.0</v>
+        <v>99.0</v>
       </c>
     </row>
     <row r="29">
@@ -1143,31 +1140,31 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="C29" t="n">
-        <v>27.0</v>
+        <v>24.0</v>
       </c>
       <c r="D29" t="n">
-        <v>9800.0</v>
+        <v>10640.0</v>
       </c>
       <c r="E29" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="F29" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="G29" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H29" t="n">
         <v>0.0</v>
       </c>
       <c r="I29" t="n">
-        <v>55.00000000000001</v>
+        <v>50.0</v>
       </c>
       <c r="J29" t="n">
-        <v>89.0</v>
+        <v>94.0</v>
       </c>
     </row>
     <row r="30">
@@ -1175,31 +1172,31 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="C30" t="n">
-        <v>21.0</v>
+        <v>34.0</v>
       </c>
       <c r="D30" t="n">
-        <v>9520.0</v>
+        <v>14000.0</v>
       </c>
       <c r="E30" t="n">
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="F30" t="n">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H30" t="n">
         <v>0.0</v>
       </c>
       <c r="I30" t="n">
-        <v>43.0</v>
+        <v>75.0</v>
       </c>
       <c r="J30" t="n">
-        <v>86.0</v>
+        <v>91.0</v>
       </c>
     </row>
     <row r="31">
@@ -1210,28 +1207,28 @@
         <v>11.0</v>
       </c>
       <c r="C31" t="n">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="D31" t="n">
-        <v>12880.0</v>
+        <v>11480.0</v>
       </c>
       <c r="E31" t="n">
         <v>11.0</v>
       </c>
       <c r="F31" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I31" t="n">
-        <v>73.0</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="J31" t="n">
-        <v>83.0</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="32">
@@ -1239,19 +1236,19 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="C32" t="n">
-        <v>62.0</v>
+        <v>65.0</v>
       </c>
       <c r="D32" t="n">
-        <v>27440.0</v>
+        <v>28280.0</v>
       </c>
       <c r="E32" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="F32" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G32" t="n">
         <v>4.0</v>
@@ -1260,10 +1257,10 @@
         <v>2.0</v>
       </c>
       <c r="I32" t="n">
-        <v>25.0</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="J32" t="n">
-        <v>73.0</v>
+        <v>81.0</v>
       </c>
     </row>
     <row r="33">
@@ -1271,19 +1268,19 @@
         <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C33" t="n">
-        <v>18.0</v>
+        <v>21.0</v>
       </c>
       <c r="D33" t="n">
-        <v>7000.0</v>
+        <v>7840.0</v>
       </c>
       <c r="E33" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G33" t="n">
         <v>0.0</v>
@@ -1292,10 +1289,10 @@
         <v>0.0</v>
       </c>
       <c r="I33" t="n">
-        <v>28.999999999999996</v>
+        <v>38.0</v>
       </c>
       <c r="J33" t="n">
-        <v>72.0</v>
+        <v>79.0</v>
       </c>
     </row>
     <row r="34">
@@ -1303,16 +1300,16 @@
         <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="C34" t="n">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
       <c r="D34" t="n">
-        <v>16601.0</v>
+        <v>17913.0</v>
       </c>
       <c r="E34" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="F34" t="n">
         <v>3.0</v>
@@ -1324,10 +1321,10 @@
         <v>0.0</v>
       </c>
       <c r="I34" t="n">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="J34" t="n">
-        <v>71.0</v>
+        <v>75.0</v>
       </c>
     </row>
     <row r="35">
@@ -1335,16 +1332,16 @@
         <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C35" t="n">
-        <v>17.0</v>
+        <v>20.0</v>
       </c>
       <c r="D35" t="n">
-        <v>7280.0</v>
+        <v>8400.0</v>
       </c>
       <c r="E35" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="F35" t="n">
         <v>3.0</v>
@@ -1356,10 +1353,10 @@
         <v>1.0</v>
       </c>
       <c r="I35" t="n">
-        <v>50.0</v>
+        <v>43.0</v>
       </c>
       <c r="J35" t="n">
-        <v>59.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="36">
@@ -1367,31 +1364,31 @@
         <v>44</v>
       </c>
       <c r="B36" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>16992.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="G36" t="n">
         <v>8.0</v>
       </c>
-      <c r="C36" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>11760.0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.0</v>
-      </c>
       <c r="H36" t="n">
         <v>1.0</v>
       </c>
       <c r="I36" t="n">
-        <v>71.0</v>
+        <v>38.0</v>
       </c>
       <c r="J36" t="n">
-        <v>52.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="37">
@@ -1399,31 +1396,31 @@
         <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="C37" t="n">
-        <v>38.0</v>
+        <v>10.0</v>
       </c>
       <c r="D37" t="n">
-        <v>16432.0</v>
+        <v>4480.0</v>
       </c>
       <c r="E37" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="F37" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="G37" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="H37" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I37" t="n">
-        <v>40.0</v>
+        <v>50.0</v>
       </c>
       <c r="J37" t="n">
-        <v>52.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="38">
@@ -1431,31 +1428,31 @@
         <v>46</v>
       </c>
       <c r="B38" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>14206.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G38" t="n">
         <v>3.0</v>
       </c>
-      <c r="C38" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>3640.0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1.0</v>
-      </c>
       <c r="H38" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I38" t="n">
-        <v>67.0</v>
+        <v>6.0</v>
       </c>
       <c r="J38" t="n">
-        <v>47.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="39">
@@ -1463,16 +1460,16 @@
         <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C39" t="n">
-        <v>19.0</v>
+        <v>22.0</v>
       </c>
       <c r="D39" t="n">
-        <v>8680.0</v>
+        <v>10360.0</v>
       </c>
       <c r="E39" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="F39" t="n">
         <v>1.0</v>
@@ -1484,10 +1481,10 @@
         <v>1.0</v>
       </c>
       <c r="I39" t="n">
-        <v>14.000000000000002</v>
+        <v>12.0</v>
       </c>
       <c r="J39" t="n">
-        <v>37.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="40">
@@ -1495,31 +1492,31 @@
         <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="C40" t="n">
-        <v>45.0</v>
+        <v>27.0</v>
       </c>
       <c r="D40" t="n">
-        <v>13069.0</v>
+        <v>13440.0</v>
       </c>
       <c r="E40" t="n">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="G40" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H40" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="J40" t="n">
-        <v>36.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="41">
@@ -1527,19 +1524,19 @@
         <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="C41" t="n">
-        <v>37.0</v>
+        <v>40.0</v>
       </c>
       <c r="D41" t="n">
-        <v>14363.0</v>
+        <v>15763.0</v>
       </c>
       <c r="E41" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G41" t="n">
         <v>2.0</v>
@@ -1548,10 +1545,10 @@
         <v>1.0</v>
       </c>
       <c r="I41" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
       <c r="J41" t="n">
-        <v>29.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="42">
@@ -1559,31 +1556,31 @@
         <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>14.0</v>
+        <v>3.0</v>
       </c>
       <c r="C42" t="n">
-        <v>29.0</v>
+        <v>9.0</v>
       </c>
       <c r="D42" t="n">
-        <v>11480.0</v>
+        <v>3920.0</v>
       </c>
       <c r="E42" t="n">
-        <v>15.0</v>
+        <v>3.0</v>
       </c>
       <c r="F42" t="n">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="G42" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="H42" t="n">
         <v>0.0</v>
       </c>
       <c r="I42" t="n">
-        <v>47.0</v>
+        <v>33.0</v>
       </c>
       <c r="J42" t="n">
-        <v>25.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="43">
@@ -1591,31 +1588,31 @@
         <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C43" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="D43" t="n">
-        <v>2450.0</v>
+        <v>1836.0</v>
       </c>
       <c r="E43" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F43" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H43" t="n">
         <v>0.0</v>
       </c>
       <c r="I43" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="J43" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="44">
@@ -1623,31 +1620,31 @@
         <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>3.0</v>
+        <v>11.0</v>
       </c>
       <c r="C44" t="n">
-        <v>5.0</v>
+        <v>26.0</v>
       </c>
       <c r="D44" t="n">
-        <v>1836.0</v>
+        <v>9868.0</v>
       </c>
       <c r="E44" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G44" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="J44" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="45">
@@ -1655,31 +1652,29 @@
         <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="C45" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="D45" t="n">
-        <v>9868.0</v>
+        <v>0.0</v>
       </c>
       <c r="E45" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="F45" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="G45" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="H45" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>20.0</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="I45"/>
       <c r="J45" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -1687,29 +1682,31 @@
         <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0</v>
+        <v>7016.0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="H46" t="n">
         <v>0.0</v>
       </c>
-      <c r="I46"/>
+      <c r="I46" t="n">
+        <v>12.0</v>
+      </c>
       <c r="J46" t="n">
-        <v>3.0</v>
+        <v>-8.0</v>
       </c>
     </row>
     <row r="47">
@@ -1717,31 +1714,29 @@
         <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="C47" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="D47" t="n">
-        <v>6281.0</v>
+        <v>0.0</v>
       </c>
       <c r="E47" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="F47" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G47" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H47" t="n">
         <v>0.0</v>
       </c>
-      <c r="I47" t="n">
-        <v>14.000000000000002</v>
-      </c>
+      <c r="I47"/>
       <c r="J47" t="n">
-        <v>-6.0</v>
+        <v>-16.0</v>
       </c>
     </row>
     <row r="48">
@@ -1749,19 +1744,19 @@
         <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0</v>
+        <v>1049.0</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G48" t="n">
         <v>0.0</v>
@@ -1769,9 +1764,11 @@
       <c r="H48" t="n">
         <v>0.0</v>
       </c>
-      <c r="I48"/>
+      <c r="I48" t="n">
+        <v>100.0</v>
+      </c>
       <c r="J48" t="n">
-        <v>-14.0</v>
+        <v>-21.0</v>
       </c>
     </row>
     <row r="49">
@@ -1779,19 +1776,19 @@
         <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C49" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D49" t="n">
-        <v>1049.0</v>
+        <v>0.0</v>
       </c>
       <c r="E49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G49" t="n">
         <v>0.0</v>
@@ -1799,11 +1796,9 @@
       <c r="H49" t="n">
         <v>0.0</v>
       </c>
-      <c r="I49" t="n">
-        <v>100.0</v>
-      </c>
+      <c r="I49"/>
       <c r="J49" t="n">
-        <v>-18.0</v>
+        <v>-36.0</v>
       </c>
     </row>
     <row r="50">
@@ -1811,61 +1806,31 @@
         <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0</v>
+        <v>9809.0</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="F50" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I50"/>
+        <v>4.0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>50.0</v>
+      </c>
       <c r="J50" t="n">
-        <v>-33.0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="C51" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="D51" t="n">
-        <v>9809.0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>-81.0</v>
+        <v>-82.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>